<commit_message>
Implement add-images with excel data logic
</commit_message>
<xml_diff>
--- a/server/random_data.xlsx
+++ b/server/random_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Desktop\New folder\tech-dose\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0B0FF6-221C-434A-8C1F-4F9FE663ABB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD898EA-F23B-4139-88EF-4C7033F222F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
   <si>
     <t>title</t>
   </si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>thumbnail1.jpg</t>
-  </si>
-  <si>
-    <t>thumbnail2.jpg</t>
   </si>
   <si>
     <t>thumbnail3.jpg</t>
@@ -582,12 +579,12 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -610,7 +607,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -621,42 +618,39 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2">
         <v>2004</v>
       </c>
       <c r="G2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3">
         <v>2022</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -664,22 +658,22 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F4">
         <v>2010</v>
       </c>
       <c r="G4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -687,22 +681,22 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5">
         <v>2003</v>
       </c>
       <c r="G5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -710,22 +704,22 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F6">
         <v>2021</v>
       </c>
       <c r="G6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -733,22 +727,22 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7">
         <v>2018</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -756,22 +750,22 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8">
         <v>2011</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -779,22 +773,22 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9">
         <v>2022</v>
       </c>
       <c r="G9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -802,22 +796,22 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F10">
         <v>2003</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -825,19 +819,19 @@
         <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F11">
         <v>2001</v>
       </c>
       <c r="G11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>